<commit_message>
Bitte Leute wenns irgendwas an der Zeitaufzeichnung änderts, dann bitte an dieser
</commit_message>
<xml_diff>
--- a/Zeitaufteilung.xlsx
+++ b/Zeitaufteilung.xlsx
@@ -185,9 +185,6 @@
     <t>Kibler,Gradonski</t>
   </si>
   <si>
-    <t>Gradonski,Kibler</t>
-  </si>
-  <si>
     <t>Novotny,Gradonski</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Benutzer anzeigen/ausgeben</t>
+  </si>
+  <si>
+    <t>Fast abgeschlossen</t>
   </si>
 </sst>
 </file>
@@ -272,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +298,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,7 +372,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -439,6 +445,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -751,11 +770,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AB42"/>
+  <dimension ref="A2:AB43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -904,7 +923,7 @@
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L6" s="24"/>
       <c r="M6" s="24"/>
@@ -935,7 +954,7 @@
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
@@ -966,7 +985,7 @@
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
@@ -978,7 +997,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="11"/>
       <c r="D9" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>29</v>
@@ -997,7 +1016,7 @@
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
@@ -1014,10 +1033,10 @@
         <v>29</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="27">
         <f>SUM(H11:H15)</f>
@@ -1025,8 +1044,8 @@
       </c>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
-      <c r="K10" s="32" t="s">
-        <v>51</v>
+      <c r="K10" s="40" t="s">
+        <v>61</v>
       </c>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
@@ -1053,8 +1072,8 @@
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
-      <c r="K11" s="32" t="s">
-        <v>51</v>
+      <c r="K11" s="40" t="s">
+        <v>61</v>
       </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
@@ -1081,8 +1100,8 @@
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="32" t="s">
-        <v>51</v>
+      <c r="K12" s="40" t="s">
+        <v>61</v>
       </c>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
@@ -1109,8 +1128,8 @@
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="32" t="s">
-        <v>51</v>
+      <c r="K13" s="40" t="s">
+        <v>61</v>
       </c>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
@@ -1121,24 +1140,24 @@
     <row r="14" spans="1:28" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="34" t="s">
         <v>48</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>52</v>
       </c>
       <c r="H14" s="13">
         <v>31</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="32" t="s">
-        <v>51</v>
+      <c r="K14" s="40" t="s">
+        <v>61</v>
       </c>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
@@ -1149,7 +1168,7 @@
     <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>31</v>
@@ -1165,8 +1184,8 @@
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="28"/>
-      <c r="K15" s="32" t="s">
-        <v>51</v>
+      <c r="K15" s="40" t="s">
+        <v>61</v>
       </c>
       <c r="L15" s="28"/>
       <c r="M15" s="13"/>
@@ -1258,10 +1277,10 @@
         <v>30</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>52</v>
       </c>
       <c r="H19" s="27">
         <f>SUM(H20)</f>
@@ -1306,79 +1325,67 @@
       <c r="O20" s="13"/>
       <c r="P20" s="13"/>
     </row>
-    <row r="21" spans="1:16" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="23" t="s">
+    <row r="21" spans="1:16" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+    </row>
+    <row r="22" spans="1:16" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24" t="s">
+      <c r="D22" s="23"/>
+      <c r="E22" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="H21" s="27">
-        <f>SUM(H22:H26)</f>
+      <c r="F22" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="27">
+        <f>SUM(H23:H27)</f>
         <v>390</v>
       </c>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="11"/>
-      <c r="D22" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H22" s="13">
-        <v>30</v>
-      </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
       <c r="K22" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-    </row>
-    <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="1"/>
-      <c r="D23" s="16" t="s">
-        <v>40</v>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="11"/>
+      <c r="D23" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F23" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G23" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="H23" s="13">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
@@ -1393,8 +1400,8 @@
     </row>
     <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
-      <c r="D24" s="20" t="s">
-        <v>41</v>
+      <c r="D24" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>29</v>
@@ -1406,7 +1413,7 @@
         <v>48</v>
       </c>
       <c r="H24" s="13">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
@@ -1422,12 +1429,12 @@
     <row r="25" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="D25" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G25" s="13" t="s">
@@ -1449,25 +1456,25 @@
     </row>
     <row r="26" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
-      <c r="D26" s="19" t="s">
-        <v>43</v>
+      <c r="D26" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>48</v>
       </c>
       <c r="H26" s="13">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
-      <c r="K26" s="29" t="s">
-        <v>50</v>
+      <c r="K26" s="32" t="s">
+        <v>51</v>
       </c>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
@@ -1475,48 +1482,56 @@
       <c r="O26" s="13"/>
       <c r="P26" s="13"/>
     </row>
-    <row r="27" spans="1:16" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="27" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="1"/>
+      <c r="D27" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="13">
+        <v>120</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+    </row>
+    <row r="28" spans="1:16" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
@@ -1531,10 +1546,11 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -1550,10 +1566,10 @@
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
@@ -1569,10 +1585,10 @@
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
@@ -1588,10 +1604,10 @@
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
@@ -1607,10 +1623,10 @@
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
@@ -1626,10 +1642,10 @@
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
@@ -1645,7 +1661,7 @@
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>29</v>
@@ -1662,27 +1678,46 @@
       <c r="O36" s="13"/>
       <c r="P36" s="13"/>
     </row>
-    <row r="37" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+    </row>
+    <row r="38" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="H37" s="9">
-        <f>SUM(H21,H19,H16,H10,H6,H27)</f>
+      <c r="E38" s="10"/>
+      <c r="H38" s="9">
+        <f>SUM(H22,H19,H16,H10,H6,H28)</f>
         <v>1322</v>
       </c>
-      <c r="I37" s="9">
-        <f>SUM(I4:I36)</f>
+      <c r="I38" s="9">
+        <f>SUM(I4:I37)</f>
         <v>580</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="15" t="s">
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="16" t="s">
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="16" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Usage-Daten hinzugefügt, Zeitaufteilung erweitert
</commit_message>
<xml_diff>
--- a/Zeitaufteilung.xlsx
+++ b/Zeitaufteilung.xlsx
@@ -441,10 +441,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -458,6 +454,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -773,8 +773,8 @@
   <dimension ref="A2:AB43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -787,30 +787,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="38" t="s">
+      <c r="G2" s="46"/>
+      <c r="H2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="38" t="s">
+      <c r="I2" s="46"/>
+      <c r="J2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="I10" s="24"/>
       <c r="J10" s="24"/>
-      <c r="K10" s="40" t="s">
+      <c r="K10" s="38" t="s">
         <v>61</v>
       </c>
       <c r="L10" s="24"/>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
-      <c r="K11" s="40" t="s">
+      <c r="K11" s="38" t="s">
         <v>61</v>
       </c>
       <c r="L11" s="13"/>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="40" t="s">
+      <c r="K12" s="38" t="s">
         <v>61</v>
       </c>
       <c r="L12" s="13"/>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="40" t="s">
+      <c r="K13" s="38" t="s">
         <v>61</v>
       </c>
       <c r="L13" s="13"/>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="40" t="s">
+      <c r="K14" s="38" t="s">
         <v>61</v>
       </c>
       <c r="L14" s="13"/>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="28"/>
-      <c r="K15" s="40" t="s">
+      <c r="K15" s="38" t="s">
         <v>61</v>
       </c>
       <c r="L15" s="28"/>
@@ -1325,21 +1325,21 @@
       <c r="O20" s="13"/>
       <c r="P20" s="13"/>
     </row>
-    <row r="21" spans="1:16" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="42"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
+    <row r="21" spans="1:16" s="39" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="40"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
       <c r="K21" s="31"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="46"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
     </row>
     <row r="22" spans="1:16" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="23" t="s">

</xml_diff>